<commit_message>
Updated 2D training schedules, no break screen
</commit_message>
<xml_diff>
--- a/conditions/schedules/train_x_first/blue_star_00/bottom_left/inputTest.xlsx
+++ b/conditions/schedules/train_x_first/blue_star_00/bottom_left/inputTest.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/giancarlodeiana/Desktop/g-casa_children_task/conditions/schedules/train_x_first/x_decreasing_steps/top_left/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\45040\Dropbox\PC (2)\Downloads\g-casa_children_task-master\g-casa_children_task-master\conditions\schedules\train_x_first\blue_star_00\bottom_left\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88C2F23D-2D9B-0C44-8C4A-65BDB4B15E49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14CD2E35-1745-4E1B-84CD-24E4D362379C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="500" windowWidth="15960" windowHeight="14620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="22">
   <si>
     <t>trialTrain</t>
   </si>
@@ -83,6 +83,9 @@
   </si>
   <si>
     <t>untrained_1D_sec_leftout</t>
+  </si>
+  <si>
+    <t>break_on_off</t>
   </si>
 </sst>
 </file>
@@ -435,15 +438,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K73"/>
+  <dimension ref="A1:L73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="N29" sqref="N29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L1" sqref="L1:L73"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -477,8 +480,11 @@
       <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L1" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -512,8 +518,11 @@
       <c r="K2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -547,8 +556,11 @@
       <c r="K3" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -582,8 +594,11 @@
       <c r="K4" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -617,8 +632,11 @@
       <c r="K5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -652,8 +670,11 @@
       <c r="K6" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -687,8 +708,11 @@
       <c r="K7" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
@@ -722,8 +746,11 @@
       <c r="K8" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
@@ -757,8 +784,11 @@
       <c r="K9" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
@@ -792,8 +822,11 @@
       <c r="K10" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
@@ -827,8 +860,11 @@
       <c r="K11" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
@@ -862,8 +898,11 @@
       <c r="K12" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>12</v>
       </c>
@@ -897,8 +936,11 @@
       <c r="K13" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>13</v>
       </c>
@@ -932,8 +974,11 @@
       <c r="K14" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>14</v>
       </c>
@@ -967,8 +1012,11 @@
       <c r="K15" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1002,8 +1050,11 @@
       <c r="K16" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1037,8 +1088,11 @@
       <c r="K17" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1072,8 +1126,11 @@
       <c r="K18" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1107,8 +1164,11 @@
       <c r="K19" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1142,8 +1202,11 @@
       <c r="K20" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1177,8 +1240,11 @@
       <c r="K21" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1212,8 +1278,11 @@
       <c r="K22" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1247,8 +1316,11 @@
       <c r="K23" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1282,8 +1354,11 @@
       <c r="K24" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1317,8 +1392,11 @@
       <c r="K25" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1352,8 +1430,11 @@
       <c r="K26" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1387,8 +1468,11 @@
       <c r="K27" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1422,8 +1506,11 @@
       <c r="K28" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1457,8 +1544,11 @@
       <c r="K29" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1492,8 +1582,11 @@
       <c r="K30" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1527,8 +1620,11 @@
       <c r="K31" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1562,8 +1658,11 @@
       <c r="K32" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1597,8 +1696,11 @@
       <c r="K33" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1632,8 +1734,11 @@
       <c r="K34" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1667,8 +1772,11 @@
       <c r="K35" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1702,8 +1810,11 @@
       <c r="K36" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>36</v>
       </c>
@@ -1737,8 +1848,11 @@
       <c r="K37" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>37</v>
       </c>
@@ -1772,8 +1886,11 @@
       <c r="K38" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>38</v>
       </c>
@@ -1807,8 +1924,11 @@
       <c r="K39" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>39</v>
       </c>
@@ -1842,8 +1962,11 @@
       <c r="K40" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>40</v>
       </c>
@@ -1877,8 +2000,11 @@
       <c r="K41" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>41</v>
       </c>
@@ -1912,8 +2038,11 @@
       <c r="K42" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>42</v>
       </c>
@@ -1947,8 +2076,11 @@
       <c r="K43" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>43</v>
       </c>
@@ -1982,8 +2114,11 @@
       <c r="K44" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>44</v>
       </c>
@@ -2017,8 +2152,11 @@
       <c r="K45" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>45</v>
       </c>
@@ -2052,8 +2190,11 @@
       <c r="K46" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>46</v>
       </c>
@@ -2087,8 +2228,11 @@
       <c r="K47" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>47</v>
       </c>
@@ -2122,8 +2266,11 @@
       <c r="K48" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>48</v>
       </c>
@@ -2157,8 +2304,11 @@
       <c r="K49" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>49</v>
       </c>
@@ -2192,8 +2342,11 @@
       <c r="K50" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>50</v>
       </c>
@@ -2227,8 +2380,11 @@
       <c r="K51" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>51</v>
       </c>
@@ -2262,8 +2418,11 @@
       <c r="K52" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>52</v>
       </c>
@@ -2297,8 +2456,11 @@
       <c r="K53" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>53</v>
       </c>
@@ -2332,8 +2494,11 @@
       <c r="K54" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A55">
         <v>54</v>
       </c>
@@ -2367,8 +2532,11 @@
       <c r="K55" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A56">
         <v>55</v>
       </c>
@@ -2402,8 +2570,11 @@
       <c r="K56" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A57">
         <v>56</v>
       </c>
@@ -2437,8 +2608,11 @@
       <c r="K57" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A58">
         <v>57</v>
       </c>
@@ -2472,8 +2646,11 @@
       <c r="K58" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A59">
         <v>58</v>
       </c>
@@ -2507,8 +2684,11 @@
       <c r="K59" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A60">
         <v>59</v>
       </c>
@@ -2542,8 +2722,11 @@
       <c r="K60" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A61">
         <v>60</v>
       </c>
@@ -2577,8 +2760,11 @@
       <c r="K61" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A62">
         <v>61</v>
       </c>
@@ -2612,8 +2798,11 @@
       <c r="K62" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A63">
         <v>62</v>
       </c>
@@ -2647,8 +2836,11 @@
       <c r="K63" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A64">
         <v>63</v>
       </c>
@@ -2682,8 +2874,11 @@
       <c r="K64" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A65">
         <v>64</v>
       </c>
@@ -2717,8 +2912,11 @@
       <c r="K65" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A66">
         <v>65</v>
       </c>
@@ -2752,8 +2950,11 @@
       <c r="K66" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A67">
         <v>66</v>
       </c>
@@ -2787,8 +2988,11 @@
       <c r="K67" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A68">
         <v>67</v>
       </c>
@@ -2822,8 +3026,11 @@
       <c r="K68" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A69">
         <v>68</v>
       </c>
@@ -2857,8 +3064,11 @@
       <c r="K69" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A70">
         <v>69</v>
       </c>
@@ -2892,8 +3102,11 @@
       <c r="K70" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A71">
         <v>70</v>
       </c>
@@ -2927,8 +3140,11 @@
       <c r="K71" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A72">
         <v>71</v>
       </c>
@@ -2962,8 +3178,11 @@
       <c r="K72" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A73">
         <v>72</v>
       </c>
@@ -2996,6 +3215,9 @@
       </c>
       <c r="K73" t="s">
         <v>12</v>
+      </c>
+      <c r="L73">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>